<commit_message>
updated  user & user error report
</commit_message>
<xml_diff>
--- a/Reports/A03 Test Results Summary Table .xlsx
+++ b/Reports/A03 Test Results Summary Table .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shivam\MS\Fall 20\AAT\A03\A03 - Full backend testing (JUnit, Jacoco, PIT)\Submission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shivam\MS\Fall 20\AAT\A03\A03 - Full backend testing (JUnit, Jacoco, PIT)\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15C18DE-3A50-4CBD-BC41-1FE58CB90013}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15007C07-DF88-4B61-B24C-6559D5CDDA39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -392,6 +392,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -409,13 +416,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,7 +758,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -775,36 +775,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="5"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
@@ -840,7 +840,7 @@
       <c r="G3" s="2">
         <v>196</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="6">
         <v>0.9</v>
       </c>
       <c r="I3" s="2">
@@ -849,7 +849,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
@@ -869,7 +869,7 @@
       <c r="G4" s="2">
         <v>196</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="6">
         <v>0.96</v>
       </c>
       <c r="I4" s="2">
@@ -1010,261 +1010,261 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.26171875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="30.26171875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="4" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="4" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="4" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>